<commit_message>
update to the final version
</commit_message>
<xml_diff>
--- a/record.xlsx
+++ b/record.xlsx
@@ -3,11 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2505" yWindow="1792" windowWidth="21600" windowHeight="11423" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="everyone" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="phoneview" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="newcandidate" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="techpass1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nontechpass1" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="techpass2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nontechpass2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ThanksList" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -56,10 +61,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -437,10 +443,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.15"/>
@@ -458,90 +464,222 @@
       </c>
       <c r="C1" s="0" t="inlineStr">
         <is>
+          <t>郵件</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
           <t>通過</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="0" t="inlineStr">
         <is>
           <t>Tammy</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>OAI</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>gamil</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>O</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="0" t="inlineStr">
         <is>
           <t>Clark</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>Tai</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="0" t="inlineStr">
         <is>
           <t>michael</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>PSI</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>O</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
         <is>
           <t>Jesicas</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>RDI</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="0" t="inlineStr">
         <is>
           <t>Happy</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>MOI</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>gamil</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>OAI</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>hotbmail</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Tai</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>hotbmail</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="n">
+        <v>789</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>PSI</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>hotbmail</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="n">
+        <v>101010</v>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>RDI</t>
+        </is>
+      </c>
+      <c r="C10" s="0" t="inlineStr">
+        <is>
+          <t>hotbmail</t>
+        </is>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>TAI</t>
+        </is>
+      </c>
+      <c r="C11" s="0" t="inlineStr">
+        <is>
+          <t>asdasdsa</t>
+        </is>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>O</t>
         </is>
@@ -559,7 +697,89 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>姓名</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>職位</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>郵件</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>通過</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>姓名</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>職位</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>郵件</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>通過</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -580,6 +800,11 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>郵件</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>通過</t>
         </is>
       </c>
@@ -587,4 +812,324 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="A2:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>姓名</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>職位</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>郵件</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>通過</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>101010</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>RDI</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>hotbmail</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="A2:F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>姓名</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>職位</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>郵件</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>通過</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Tammy</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>OAI</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>gamil</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Happy</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MOI</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>gamil</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>123</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>OAI</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>hotbmail</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>姓名</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>職位</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>郵件</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>通過</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="1">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>Clark</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Tai</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>Jesicas</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>RDI</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="n">
+        <v>456</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Tai</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>hotbmail</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>TAI</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>asdasdsa</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>michael</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PSI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>yahoo</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>789</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>PSI</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>hotbmail</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>